<commit_message>
update study end estimate including new accruals
</commit_message>
<xml_diff>
--- a/data/derived/mitox-patient-consent-dates.xlsx
+++ b/data/derived/mitox-patient-consent-dates.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11108"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wil407\Box Sync\mitox\protocols\mitox-protocol\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielspakowicz/Documents/GitHub/mitox/data/derived/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783D3848-728D-A940-9A21-2E5E3AC9E7D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11080"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="11080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>M001</t>
   </si>
@@ -105,12 +106,21 @@
   </si>
   <si>
     <t>Record Id</t>
+  </si>
+  <si>
+    <t>M033</t>
+  </si>
+  <si>
+    <t>M030</t>
+  </si>
+  <si>
+    <t>M031</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -154,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -173,6 +183,12 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -453,20 +469,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A19" sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6328125" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -474,7 +490,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>43871</v>
       </c>
@@ -482,7 +498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>43878</v>
       </c>
@@ -490,7 +506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>43878</v>
       </c>
@@ -498,7 +514,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>43880</v>
       </c>
@@ -506,7 +522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44040</v>
       </c>
@@ -514,7 +530,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>44018</v>
       </c>
@@ -522,7 +538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>44019</v>
       </c>
@@ -530,7 +546,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>44026</v>
       </c>
@@ -538,7 +554,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44054</v>
       </c>
@@ -546,7 +562,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44062</v>
       </c>
@@ -554,7 +570,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>44068</v>
       </c>
@@ -562,7 +578,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>44068</v>
       </c>
@@ -570,7 +586,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>44068</v>
       </c>
@@ -578,7 +594,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>44069</v>
       </c>
@@ -586,7 +602,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>44070</v>
       </c>
@@ -594,7 +610,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>44074</v>
       </c>
@@ -602,7 +618,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>44082</v>
       </c>
@@ -610,7 +626,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>44085</v>
       </c>
@@ -618,7 +634,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>44089</v>
       </c>
@@ -626,7 +642,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>44089</v>
       </c>
@@ -634,7 +650,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>44090</v>
       </c>
@@ -642,7 +658,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>44090</v>
       </c>
@@ -650,7 +666,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>44096</v>
       </c>
@@ -658,7 +674,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>44109</v>
       </c>
@@ -666,12 +682,36 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>44125</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="7">
+        <v>44159</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="7">
+        <v>44159</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="7">
+        <v>44166</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>